<commit_message>
Modified use cases Template
</commit_message>
<xml_diff>
--- a/documentation/Use Case Template.xlsx
+++ b/documentation/Use Case Template.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{934F4DFB-AD88-471B-9E0E-62A6C48B6297}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpaces\SoftWareEngineering\senteApp\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32A879-A14F-4BEC-B4B2-7749687B0410}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Use Case Number</t>
   </si>
@@ -46,18 +51,12 @@
     <t>Basic Flows</t>
   </si>
   <si>
-    <t>Flow 1</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
     <t>User Actions</t>
   </si>
   <si>
-    <t>System Actions</t>
-  </si>
-  <si>
     <t>Alternate Flows</t>
   </si>
   <si>
@@ -65,15 +64,56 @@
   </si>
   <si>
     <t>Business Rules</t>
+  </si>
+  <si>
+    <t>Second Member</t>
+  </si>
+  <si>
+    <t>Group Member</t>
+  </si>
+  <si>
+    <t>This use case allows a member to stand surety of another member taking out a laon</t>
+  </si>
+  <si>
+    <t>System Response</t>
+  </si>
+  <si>
+    <t>The group member selects the approval tab</t>
+  </si>
+  <si>
+    <t>The system displays all the pending approvals for the group member</t>
+  </si>
+  <si>
+    <t>The group member selects the transactions they want to approve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system updates the database </t>
+  </si>
+  <si>
+    <t>In case a member does not want to second another member, he clicks the reject button and the system notifies the member seeking a loan</t>
+  </si>
+  <si>
+    <t>Member seconded succesfully</t>
+  </si>
+  <si>
+    <t>1.Group Member has logged in to the system
+2. Group Member has been selected to be a seconder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -88,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -112,19 +152,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -159,26 +186,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -238,21 +245,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,166 +624,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="34.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="1" t="s">
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="7"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="4" t="s">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D9" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="13"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
       <c r="C19" s="11"/>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="9"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="9"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3"/>
-    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B7:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Added document with Kedi Use cases and updated the excel template with a second sheet containing Kedi Use Cases in excel.
</commit_message>
<xml_diff>
--- a/documentation/Use Case Template.xlsx
+++ b/documentation/Use Case Template.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpaces\SoftWareEngineering\senteApp\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new/Documents/SoftwareEngineering/WorkSpace/Project/senteApp/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32A879-A14F-4BEC-B4B2-7749687B0410}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kedi" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Use Case Number</t>
   </si>
@@ -98,12 +101,143 @@
   <si>
     <t>1.Group Member has logged in to the system
 2. Group Member has been selected to be a seconder</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>A use case for a user Login</t>
+  </si>
+  <si>
+    <t>Group Member / Admin / Account Manager</t>
+  </si>
+  <si>
+    <t>1.Access to the internet or local network and a device.</t>
+  </si>
+  <si>
+    <t>The application opens up.</t>
+  </si>
+  <si>
+    <t>The user supplies login details, both user name and password.</t>
+  </si>
+  <si>
+    <t>The system checks to see if the user exists in the system and validates the supplied password against the stored logins and opens up the respective GUI that corresponds to the user's role type.</t>
+  </si>
+  <si>
+    <t>1. Incase the user supplies the wrong username, the system responds with user doesn’t exist.
+2. Incase the user supplies a correct username but with a wrong password, system responds with "incorrect password" message.</t>
+  </si>
+  <si>
+    <t>User Logged in successful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User details should exist in the system.
+2. Every user should have a specific role type , ie Member, Admin, Account Manager
+</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>A use case for a user Logout</t>
+  </si>
+  <si>
+    <t>User should be logged-in.</t>
+  </si>
+  <si>
+    <t>The user opens the application on his/her device.</t>
+  </si>
+  <si>
+    <t>The user goes under settings and taps on logout /signout button</t>
+  </si>
+  <si>
+    <t>The system closes the current session</t>
+  </si>
+  <si>
+    <t>User Logged - out successful.</t>
+  </si>
+  <si>
+    <t>System looks up the user session ID and terminates.</t>
+  </si>
+  <si>
+    <t>Make Deposits</t>
+  </si>
+  <si>
+    <t>A use case for member deposits</t>
+  </si>
+  <si>
+    <t>1. User should be logged-in.</t>
+  </si>
+  <si>
+    <t>Under the member dashboard, the member taps on the deposit button.</t>
+  </si>
+  <si>
+    <t>System opens a page with an input field requesting how much they want to deposit and a pay button below that.</t>
+  </si>
+  <si>
+    <t>Member inputs how much they want to pay, and then submits.</t>
+  </si>
+  <si>
+    <t>System picks up the amount and then opens up a payment plugin modal, with options of pay with card or pay with mobile number and the different fields for  both options.</t>
+  </si>
+  <si>
+    <t>Member chooses the payment option they want to use and supplies the required information and submits information</t>
+  </si>
+  <si>
+    <t>System takes supplied information and validates it with the payment gateway API.</t>
+  </si>
+  <si>
+    <t>1. If user provides an amount that is less than the minimum deposit, system responds with " Please provide an amount bigger than $XXX".
+2. If User provides wrong Card card details, system responds with "Please provide correct card details"
+3. If user provides wrong mobile number , system responds with "Invalid mobile number".
+4. If user provides a number with unsufficient funds to what he wants to deposit to the App, system responds with "Account has insuffucient funds"
+5. If user provides card with insuffucient funds, system responds with "card cannot be billed".</t>
+  </si>
+  <si>
+    <t>User has succesfully deposited.</t>
+  </si>
+  <si>
+    <t>1. System validates deposit amount so that its more than the minimum deposit.
+2. System validates input mobile number format.
+3. System validates the input card details format.
+4. System checks if the mobile number has enough funds for deposit.
+5. System checks if the card has enough funds for deposit.</t>
+  </si>
+  <si>
+    <t>View Statements</t>
+  </si>
+  <si>
+    <t>A use case for a member to view his or her statements</t>
+  </si>
+  <si>
+    <t>Under the member dashboard, the member taps on the view statement button.</t>
+  </si>
+  <si>
+    <t>System opens a page with an opens a page with fields to be filled, including Month,Year and a submit button</t>
+  </si>
+  <si>
+    <t>Member fills the fields with a month and year of their choice whose statement he/she wants to view and taps submit.</t>
+  </si>
+  <si>
+    <t>System responds with a details for the given values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. If user provides an a year or month whose statement is not contained in the System, system responds with a page "No Statement Found".
+2. If User provides wrong field value formats System responds with "Please provide valid Year /Month".
+</t>
+  </si>
+  <si>
+    <t>User's Statement successfully retrieved.</t>
+  </si>
+  <si>
+    <t>1. System validates input value formats.
+2. System checks if the supplied year and month exist for a given user requesting.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -256,12 +390,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -277,37 +447,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -623,157 +769,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="34.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="34.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
         <v>2</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="21" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="C16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="D16" s="16"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -789,4 +935,659 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67:D67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="2:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="2:4" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15">
+        <v>2</v>
+      </c>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="13"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="8"/>
+      <c r="C36" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="16"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="8"/>
+      <c r="C39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="16"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="15">
+        <v>3</v>
+      </c>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="24"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="21"/>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="B50" s="6">
+        <v>2</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="B51" s="6">
+        <v>3</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="10"/>
+    </row>
+    <row r="54" spans="2:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="6">
+        <v>1</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="16"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="13"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="8"/>
+      <c r="C57" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="16"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="1"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="2:4" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="8"/>
+      <c r="C60" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="16"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="15">
+        <v>4</v>
+      </c>
+      <c r="D62" s="16"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" s="16"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="16"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="24"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="16"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="21"/>
+      <c r="D67" s="22"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="B70" s="6">
+        <v>1</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="B71" s="6">
+        <v>2</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="6"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="2:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="6">
+        <v>1</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" s="16"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="13"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" s="8"/>
+      <c r="C77" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" s="16"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="1"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="8"/>
+      <c r="C80" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added SRS Document with all use cases
</commit_message>
<xml_diff>
--- a/documentation/Use Case Template.xlsx
+++ b/documentation/Use Case Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpaces\SoftWareEngineering\senteApp\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\610096\Documents\senteApp\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32A879-A14F-4BEC-B4B2-7749687B0410}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F1946B-A79C-43E5-8B01-1FDF470B332F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Use Case Number</t>
   </si>
@@ -57,54 +57,133 @@
     <t>User Actions</t>
   </si>
   <si>
-    <t>Alternate Flows</t>
-  </si>
-  <si>
     <t>Post Conditions</t>
   </si>
   <si>
     <t>Business Rules</t>
   </si>
   <si>
-    <t>Second Member</t>
-  </si>
-  <si>
-    <t>Group Member</t>
-  </si>
-  <si>
-    <t>This use case allows a member to stand surety of another member taking out a laon</t>
-  </si>
-  <si>
     <t>System Response</t>
   </si>
   <si>
-    <t>The group member selects the approval tab</t>
-  </si>
-  <si>
-    <t>The system displays all the pending approvals for the group member</t>
-  </si>
-  <si>
-    <t>The group member selects the transactions they want to approve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system updates the database </t>
-  </si>
-  <si>
-    <t>In case a member does not want to second another member, he clicks the reject button and the system notifies the member seeking a loan</t>
-  </si>
-  <si>
-    <t>Member seconded succesfully</t>
-  </si>
-  <si>
-    <t>1.Group Member has logged in to the system
-2. Group Member has been selected to be a seconder</t>
+    <t>Generate Report</t>
+  </si>
+  <si>
+    <t>This use case allows a member to generate a report for a selected period. If a member is an account manager he will be able to generate report for the entire group</t>
+  </si>
+  <si>
+    <t>Group Member, Account Manager</t>
+  </si>
+  <si>
+    <t>The group member selects the generate report tab and chooses a period range</t>
+  </si>
+  <si>
+    <t>The system displays a summary of all the transactions executed by the member in that period</t>
+  </si>
+  <si>
+    <t>The member then can now choose to print or email the statement</t>
+  </si>
+  <si>
+    <t>The system responds by either sending a mail or provide options for printing the statement</t>
+  </si>
+  <si>
+    <t>The system records this event for persistence either in a logFile or in the DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Member has logged in to the system
+</t>
+  </si>
+  <si>
+    <t>Member management CRUD</t>
+  </si>
+  <si>
+    <t>Account Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Manager has logged in to the system
+</t>
+  </si>
+  <si>
+    <t>Create Member</t>
+  </si>
+  <si>
+    <t>The manager calls the create member command</t>
+  </si>
+  <si>
+    <t>The system presents a form with fields including email, dateOfBirth, dateOfJoing, Names and Address</t>
+  </si>
+  <si>
+    <t>The manager then requests the system to save member details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system responds by validating input and checking if this member already exists. Then finally adds member to that account </t>
+  </si>
+  <si>
+    <t>1. The system displays a toast or message confirming to the admin the member has been succesful or unsuccesful added. 
+2.The system records this event for persistence either in a logFile or in the DB2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The member must have a unique ID </t>
+  </si>
+  <si>
+    <t>Edit Member</t>
+  </si>
+  <si>
+    <t>Read/View Member</t>
+  </si>
+  <si>
+    <t>The manager requests to view a list of members</t>
+  </si>
+  <si>
+    <t>The system presents a list of all members</t>
+  </si>
+  <si>
+    <t>The manager then chooses one member whose details he desires to edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system then presents a form with existing member details </t>
+  </si>
+  <si>
+    <t>The manager then edits the member information as he wishes and clicks the save button</t>
+  </si>
+  <si>
+    <t>The system then validates input and overrites member info with updated info</t>
+  </si>
+  <si>
+    <t>Approve Member Exit Request</t>
+  </si>
+  <si>
+    <t>1.Account Manager has logged in to the system
+2.There should be a request from member to exit</t>
+  </si>
+  <si>
+    <t>1. The system displays a toast or message confirming to the manager that the member has been disabled 
+2.The system records this event for persistence either in a logFile or in the DB2.</t>
+  </si>
+  <si>
+    <t>The manager clicks on disable button</t>
+  </si>
+  <si>
+    <t>The system responds by changing the active status to false</t>
+  </si>
+  <si>
+    <t>The member must have cleared all his outstanding loans</t>
+  </si>
+  <si>
+    <t>The manager calls the view member command</t>
+  </si>
+  <si>
+    <t>The system presents a statement with members details</t>
+  </si>
+  <si>
+    <t>The member unique ID cannot be edited</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +198,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -202,15 +289,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -232,20 +310,92 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -256,59 +406,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,17 +822,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="34.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -642,143 +841,482 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5"/>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="7"/>
+      <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5"/>
+      <c r="C6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+      <c r="C18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="2:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="C19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="18">
+        <v>1</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="18">
+        <v>2</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="C29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="18">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="C34" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="18">
+        <v>2</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="18">
+        <v>3</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="2:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="20"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="C39" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="20"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
+    </row>
+    <row r="43" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="18">
+        <v>1</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="24"/>
+    </row>
+    <row r="45" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="20"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="27"/>
+    </row>
+    <row r="49" spans="2:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="20"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="24"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="18">
+        <v>1</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="22"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="2:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="20"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="20"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="36">
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C5:D5"/>

</xml_diff>

<commit_message>
modified:   documentation/Use Case Template.xlsx deleted:    documentation/~ Case Template.xlsx documentation/SRS Document.docx documentation/System Architecture .pdf
</commit_message>
<xml_diff>
--- a/documentation/Use Case Template.xlsx
+++ b/documentation/Use Case Template.xlsx
@@ -238,7 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +249,28 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,8 +398,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -457,7 +483,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -939,655 +969,657 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D80"/>
+  <dimension ref="A3:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:D67"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" spans="2:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="15">
+        <v>2</v>
+      </c>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="75" x14ac:dyDescent="0.2">
-      <c r="B12" s="8">
+      <c r="B30" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="16"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="15">
+        <v>3</v>
+      </c>
+      <c r="C41" s="16"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="16"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="11" t="s">
+      <c r="B43" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="16"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="24"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="16"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="21"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>1</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>2</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>3</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="2:4" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6">
+      <c r="B53" s="12"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="B54" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="16"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
-      <c r="C17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+      <c r="B57" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="16"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="16"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="1:3" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="16"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="15">
+      <c r="B62" s="15">
+        <v>4</v>
+      </c>
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="16"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="16"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+      <c r="B64" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" s="16"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="24"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="16"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="22"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
         <v>1</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="B70" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
         <v>2</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="16"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B30" s="6">
+      <c r="B71" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="6"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
         <v>1</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="6">
-        <v>1</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="13"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+      <c r="B74" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="16"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="13"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="8"/>
-      <c r="C36" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="16"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
+      <c r="B76" s="9"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="8"/>
+      <c r="B77" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" s="16"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="8"/>
-      <c r="C39" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="16"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="15">
-        <v>3</v>
-      </c>
-      <c r="D41" s="16"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="16"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="24"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="16"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="22"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B49" s="6">
-        <v>1</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="B50" s="6">
-        <v>2</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="B51" s="6">
-        <v>3</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="2:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="6">
-        <v>1</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="16"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="13"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="8"/>
-      <c r="C57" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="16"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="2:4" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="8"/>
-      <c r="C60" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="16"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="15">
-        <v>4</v>
-      </c>
-      <c r="D62" s="16"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D63" s="16"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D64" s="16"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="24"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D66" s="16"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="21"/>
-      <c r="D67" s="22"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B68" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B70" s="6">
-        <v>1</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="B71" s="6">
-        <v>2</v>
-      </c>
-      <c r="C71" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="6"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="7"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B73" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="2:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="6">
-        <v>1</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D74" s="16"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="13"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B77" s="8"/>
-      <c r="C77" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77" s="16"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B78" s="1"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79" s="9"/>
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="8"/>
-      <c r="C80" s="15" t="s">
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+    </row>
+    <row r="80" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="8"/>
+      <c r="B80" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D80" s="16"/>
+      <c r="C80" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>